<commit_message>
base Employee class and specialized Freelancer class
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Freelancer</t>
+          <t>Employee</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -560,24 +560,24 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -696,29 +696,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -798,24 +798,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -922,24 +922,24 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1065,17 +1065,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1235,17 +1235,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1405,12 +1405,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1495,12 +1495,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1558,17 +1558,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1580,12 +1580,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1597,12 +1597,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1660,17 +1660,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1728,12 +1728,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1750,12 +1750,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1796,17 +1796,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1852,29 +1852,29 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1886,24 +1886,24 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1920,12 +1920,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1937,24 +1937,24 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2000,17 +2000,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2022,12 +2022,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2039,12 +2039,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2056,29 +2056,29 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2107,12 +2107,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2124,29 +2124,29 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2192,12 +2192,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2209,12 +2209,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2323,17 +2323,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2345,12 +2345,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2362,12 +2362,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2379,12 +2379,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2430,12 +2430,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2476,17 +2476,17 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2498,12 +2498,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2515,12 +2515,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2566,12 +2566,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2612,17 +2612,17 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2651,12 +2651,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2668,12 +2668,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2719,12 +2719,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2765,17 +2765,17 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2804,12 +2804,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2821,12 +2821,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2838,12 +2838,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2884,17 +2884,17 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2923,12 +2923,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2986,17 +2986,17 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3054,12 +3054,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3076,12 +3076,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3093,12 +3093,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3122,17 +3122,17 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3161,12 +3161,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3195,29 +3195,29 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3280,29 +3280,29 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3331,12 +3331,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3365,24 +3365,24 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3433,12 +3433,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3513,12 +3513,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3569,12 +3569,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3586,12 +3586,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3637,27 +3637,10 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C190" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>

</xml_diff>

<commit_message>
splitting UI/Logic, moving build into seperate folder
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -572,34 +572,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -708,34 +708,34 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -798,46 +798,46 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -917,24 +917,24 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -946,17 +946,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1053,41 +1053,41 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1223,46 +1223,46 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1393,24 +1393,24 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1422,17 +1422,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1495,12 +1495,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1546,41 +1546,41 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1648,46 +1648,46 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1716,24 +1716,24 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1745,17 +1745,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1784,41 +1784,41 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1881,7 +1881,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1908,24 +1908,24 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1949,29 +1949,29 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2000,34 +2000,34 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2056,41 +2056,41 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2136,12 +2136,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2153,12 +2153,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2192,12 +2192,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2226,12 +2226,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2277,12 +2277,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2294,12 +2294,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2311,46 +2311,46 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2379,12 +2379,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2396,12 +2396,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2447,12 +2447,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2464,46 +2464,46 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2515,12 +2515,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2583,12 +2583,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2600,41 +2600,41 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2736,12 +2736,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2753,41 +2753,41 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2872,41 +2872,41 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2940,12 +2940,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2957,12 +2957,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2974,46 +2974,46 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3042,24 +3042,24 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3071,17 +3071,17 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3110,41 +3110,41 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3178,12 +3178,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3195,24 +3195,24 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3224,12 +3224,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3263,12 +3263,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3280,24 +3280,24 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3309,12 +3309,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3348,12 +3348,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3365,46 +3365,46 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3416,12 +3416,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3433,12 +3433,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3467,12 +3467,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3484,12 +3484,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3501,24 +3501,24 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3530,17 +3530,17 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3552,12 +3552,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3569,12 +3569,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3603,12 +3603,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3620,12 +3620,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3637,10 +3637,44 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
           <t>Paul(F)</t>
         </is>
       </c>
-      <c r="C189" t="inlineStr">
+      <c r="C191" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>

</xml_diff>

<commit_message>
error message for understaffed(assigning logic still bugged)
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -832,24 +832,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -956,24 +956,24 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -985,12 +985,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1099,17 +1099,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1269,17 +1269,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1439,12 +1439,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1478,12 +1478,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1592,17 +1592,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1648,12 +1648,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1665,12 +1665,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1682,24 +1682,24 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1711,7 +1711,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1721,19 +1721,19 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1745,7 +1745,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1755,104 +1755,104 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1864,29 +1864,29 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1898,12 +1898,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1915,29 +1915,29 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1949,24 +1949,24 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1993,19 +1993,19 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2017,41 +2017,41 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2061,31 +2061,31 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2095,14 +2095,14 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2119,24 +2119,24 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2146,14 +2146,14 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2170,24 +2170,24 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2204,12 +2204,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2221,12 +2221,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2238,7 +2238,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2248,19 +2248,19 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2272,12 +2272,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2289,216 +2289,216 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2510,63 +2510,63 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2578,29 +2578,29 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2612,12 +2612,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2629,97 +2629,97 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2731,63 +2731,63 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2799,29 +2799,29 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -2833,12 +2833,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2850,12 +2850,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2867,80 +2867,80 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2952,12 +2952,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2969,46 +2969,46 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3020,41 +3020,41 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -3064,19 +3064,19 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3088,63 +3088,63 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3156,63 +3156,63 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3224,12 +3224,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3241,12 +3241,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3258,29 +3258,29 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3292,24 +3292,24 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -3326,12 +3326,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3343,7 +3343,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3353,36 +3353,36 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3394,12 +3394,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3411,46 +3411,46 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3462,12 +3462,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3479,29 +3479,29 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3513,29 +3513,29 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3547,136 +3547,1105 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-04-09</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>10-19</t>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>7-16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
schedule_gen with senior editor, test logic in scheduling_logic (add employee)
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C248"/>
+  <dimension ref="A1:C291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -606,17 +606,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -730,63 +730,63 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,68 +861,68 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -980,7 +980,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -997,12 +997,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1014,7 +1014,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1024,14 +1024,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1041,121 +1041,121 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1167,7 +1167,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1177,14 +1177,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1201,7 +1201,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1211,14 +1211,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1228,14 +1228,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1286,12 +1286,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1303,24 +1303,24 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1330,48 +1330,48 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1388,80 +1388,80 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1473,63 +1473,63 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1541,46 +1541,46 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1592,63 +1592,63 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1660,160 +1660,160 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1823,19 +1823,19 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1847,58 +1847,58 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1908,138 +1908,138 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2051,182 +2051,182 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2238,29 +2238,29 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2282,121 +2282,121 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2408,12 +2408,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2425,97 +2425,97 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2527,12 +2527,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2544,7 +2544,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2554,82 +2554,82 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2639,14 +2639,14 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2663,41 +2663,41 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2707,48 +2707,48 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2758,14 +2758,14 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2775,14 +2775,14 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2792,14 +2792,14 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2809,14 +2809,14 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2833,7 +2833,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2843,19 +2843,19 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2867,12 +2867,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2884,63 +2884,63 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2952,46 +2952,46 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3003,12 +3003,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3020,12 +3020,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3037,29 +3037,29 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3071,12 +3071,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3088,12 +3088,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3105,46 +3105,46 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3156,24 +3156,24 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3183,19 +3183,19 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3207,63 +3207,63 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3275,12 +3275,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3292,12 +3292,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3309,46 +3309,46 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3360,12 +3360,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3377,24 +3377,24 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -3404,19 +3404,19 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3428,97 +3428,97 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3530,12 +3530,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3547,24 +3547,24 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -3581,80 +3581,80 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3666,29 +3666,29 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3700,12 +3700,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3717,63 +3717,63 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -3785,12 +3785,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -3802,29 +3802,29 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3836,12 +3836,12 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3853,24 +3853,24 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -3880,31 +3880,31 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -3914,48 +3914,48 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -3965,53 +3965,53 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -4023,12 +4023,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -4040,29 +4040,29 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -4074,63 +4074,63 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -4142,12 +4142,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4159,29 +4159,29 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4193,24 +4193,24 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4227,7 +4227,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4237,31 +4237,31 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -4271,36 +4271,36 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4312,46 +4312,46 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4363,29 +4363,29 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4397,29 +4397,29 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -4431,12 +4431,12 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -4448,12 +4448,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -4465,24 +4465,24 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -4492,121 +4492,121 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -4618,7 +4618,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4628,24 +4628,755 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B248" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C248" t="inlineStr">
-        <is>
-          <t>7-16</t>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>13-22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add, edit employee & UI update for these functions (delete bugged)
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C291"/>
+  <dimension ref="A1:C301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,17 +623,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -781,46 +781,46 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -917,24 +917,24 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -946,34 +946,34 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,12 +1002,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1070,12 +1070,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1104,24 +1104,24 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1133,46 +1133,46 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1240,12 +1240,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1274,12 +1274,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1308,41 +1308,41 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1354,12 +1354,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1371,34 +1371,34 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1495,58 +1495,58 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1558,51 +1558,51 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1665,12 +1665,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1682,41 +1682,41 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1728,12 +1728,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1745,12 +1745,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1762,51 +1762,51 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1835,12 +1835,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1852,41 +1852,41 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1898,102 +1898,102 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2005,12 +2005,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2022,41 +2022,41 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2068,24 +2068,24 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2102,7 +2102,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2119,7 +2119,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2136,7 +2136,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2153,7 +2153,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2170,29 +2170,29 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2204,41 +2204,41 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2255,7 +2255,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2289,7 +2289,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2306,7 +2306,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2323,12 +2323,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2357,12 +2357,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2374,41 +2374,41 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2418,14 +2418,14 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2442,7 +2442,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2459,7 +2459,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2476,7 +2476,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2493,7 +2493,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2503,104 +2503,104 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2612,97 +2612,97 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2724,53 +2724,53 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2782,24 +2782,24 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2816,7 +2816,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2833,41 +2833,41 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2877,65 +2877,65 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2952,24 +2952,24 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -2979,14 +2979,14 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2996,31 +2996,31 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -3030,19 +3030,19 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3054,24 +3054,24 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -3081,14 +3081,14 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -3105,7 +3105,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -3122,7 +3122,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -3139,7 +3139,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -3156,7 +3156,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -3173,7 +3173,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3190,7 +3190,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3207,7 +3207,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -3217,14 +3217,14 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3241,7 +3241,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3258,24 +3258,24 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3285,31 +3285,31 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -3319,14 +3319,14 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -3336,58 +3336,58 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3416,12 +3416,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3433,12 +3433,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3467,12 +3467,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3484,41 +3484,41 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3530,12 +3530,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3547,12 +3547,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3564,29 +3564,29 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3598,12 +3598,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3615,51 +3615,51 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3671,12 +3671,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3688,12 +3688,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3705,12 +3705,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3722,41 +3722,41 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3768,7 +3768,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -3785,7 +3785,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3802,7 +3802,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -3819,7 +3819,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -3836,7 +3836,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -3853,7 +3853,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -3870,7 +3870,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -3887,7 +3887,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -3904,7 +3904,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -3914,48 +3914,48 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -3965,14 +3965,14 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -3982,31 +3982,31 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -4016,19 +4016,19 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -4040,7 +4040,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -4050,24 +4050,24 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4079,19 +4079,19 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -4101,65 +4101,65 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -4176,7 +4176,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -4193,7 +4193,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4227,7 +4227,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4244,7 +4244,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -4261,7 +4261,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -4278,7 +4278,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -4295,7 +4295,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4312,41 +4312,41 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -4356,19 +4356,19 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4380,7 +4380,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -4390,53 +4390,53 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -4448,12 +4448,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -4465,46 +4465,46 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4516,29 +4516,29 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -4550,12 +4550,12 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -4567,182 +4567,182 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4754,12 +4754,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4771,29 +4771,29 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -4805,29 +4805,29 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -4839,63 +4839,63 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -4907,63 +4907,63 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4975,80 +4975,80 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -5060,80 +5060,80 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -5145,24 +5145,24 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -5179,7 +5179,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -5196,7 +5196,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -5213,7 +5213,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -5230,7 +5230,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -5247,7 +5247,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -5264,7 +5264,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -5281,7 +5281,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -5298,7 +5298,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -5315,7 +5315,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -5332,7 +5332,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -5349,7 +5349,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -5366,15 +5366,185 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Daisy(S)</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>13-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B291" t="inlineStr">
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
         <is>
           <t>Daisy(S)</t>
         </is>
       </c>
-      <c r="C291" t="inlineStr">
+      <c r="C301" t="inlineStr">
         <is>
           <t>13-22</t>
         </is>

</xml_diff>

<commit_message>
fixing bugs: freelancer schedule generate
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit employee working and refreshing UI
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C304"/>
+  <dimension ref="A1:C312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,7 +628,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -674,51 +674,51 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -849,24 +849,24 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -878,46 +878,46 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -929,12 +929,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -968,12 +968,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -985,12 +985,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1014,85 +1014,85 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1172,12 +1172,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1206,58 +1206,58 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1269,34 +1269,34 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1410,12 +1410,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1427,41 +1427,41 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1473,12 +1473,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1490,29 +1490,29 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1580,12 +1580,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1631,24 +1631,24 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1660,29 +1660,29 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1694,34 +1694,34 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1767,12 +1767,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1784,12 +1784,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1818,12 +1818,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1835,97 +1835,97 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1937,12 +1937,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1954,12 +1954,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1971,12 +1971,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2005,12 +2005,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2022,24 +2022,24 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2051,29 +2051,29 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2085,34 +2085,34 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2141,12 +2141,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2158,7 +2158,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2192,12 +2192,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2209,58 +2209,58 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2272,34 +2272,34 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2311,12 +2311,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2345,12 +2345,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2362,24 +2362,24 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2391,68 +2391,68 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2481,12 +2481,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2498,12 +2498,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2515,12 +2515,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2544,29 +2544,29 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2578,51 +2578,51 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2668,12 +2668,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2685,12 +2685,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2702,58 +2702,58 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2765,7 +2765,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2775,87 +2775,87 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Test1(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2867,29 +2867,29 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2901,24 +2901,24 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2928,24 +2928,24 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -2957,121 +2957,121 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -3081,24 +3081,24 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3110,36 +3110,36 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -3156,24 +3156,24 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3183,14 +3183,14 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3200,31 +3200,31 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3234,24 +3234,24 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3275,12 +3275,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3292,12 +3292,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3309,29 +3309,29 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3343,7 +3343,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3353,19 +3353,19 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3377,34 +3377,34 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3416,12 +3416,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3433,24 +3433,24 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3462,12 +3462,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3479,12 +3479,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3496,85 +3496,85 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3586,12 +3586,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3603,12 +3603,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3620,12 +3620,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3671,12 +3671,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3688,12 +3688,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3705,92 +3705,92 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -3802,51 +3802,51 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3909,12 +3909,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3926,12 +3926,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3943,41 +3943,41 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -3989,7 +3989,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -3999,19 +3999,19 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -4023,68 +4023,68 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4096,12 +4096,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -4113,126 +4113,126 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4244,17 +4244,17 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4266,12 +4266,12 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -4283,12 +4283,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -4300,148 +4300,148 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4453,7 +4453,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -4470,24 +4470,24 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4499,12 +4499,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4516,41 +4516,41 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4560,19 +4560,19 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4594,24 +4594,24 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4623,19 +4623,19 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -4645,14 +4645,14 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4669,46 +4669,46 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4720,7 +4720,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -4730,53 +4730,53 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4788,58 +4788,58 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -4849,48 +4849,48 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -4907,7 +4907,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -4924,7 +4924,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -4934,14 +4934,14 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -4958,7 +4958,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -4975,7 +4975,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -4985,14 +4985,14 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -5009,7 +5009,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -5026,7 +5026,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -5043,7 +5043,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -5077,7 +5077,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -5111,7 +5111,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -5145,7 +5145,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -5162,7 +5162,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -5179,7 +5179,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -5196,12 +5196,12 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -5213,24 +5213,24 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -5240,48 +5240,48 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -5298,41 +5298,41 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -5349,51 +5349,51 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -5405,12 +5405,12 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -5422,58 +5422,58 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -5485,85 +5485,85 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Daisy(S)</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -5575,12 +5575,12 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -5592,10 +5592,146 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
+          <t>Helen(F)</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Lili(F)</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Matthew(F)</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Ka(F)</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Kit(F)</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Paul(F)</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
           <t>Daisy(S)</t>
         </is>
       </c>
-      <c r="C304" t="inlineStr">
+      <c r="C312" t="inlineStr">
         <is>
           <t>13-22</t>
         </is>

</xml_diff>

<commit_message>
bug fix: working scheduling logic after role changing
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C312"/>
+  <dimension ref="A1:C296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -674,51 +674,51 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -883,63 +883,63 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1065,34 +1065,34 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1240,12 +1240,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1257,41 +1257,41 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1478,41 +1478,41 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1563,12 +1563,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1597,12 +1597,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1631,12 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1648,12 +1648,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1665,12 +1665,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1682,46 +1682,46 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1801,12 +1801,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1835,12 +1835,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1852,12 +1852,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1869,12 +1869,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1886,12 +1886,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1903,29 +1903,29 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1954,12 +1954,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2005,12 +2005,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2090,12 +2090,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2277,12 +2277,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2430,24 +2430,24 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2481,12 +2481,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2583,12 +2583,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2600,29 +2600,29 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2702,12 +2702,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2787,12 +2787,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2804,12 +2804,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>test1(F)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2821,29 +2821,29 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Test1(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2935,17 +2935,17 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2957,12 +2957,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3042,12 +3042,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3088,17 +3088,17 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3132,7 +3132,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3144,7 +3144,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3195,12 +3195,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>test2(F)</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3241,17 +3241,17 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3263,12 +3263,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3297,12 +3297,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3348,12 +3348,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3370,41 +3370,41 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3518,63 +3518,63 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -3637,12 +3637,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3654,12 +3654,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3671,12 +3671,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3688,12 +3688,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3739,12 +3739,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3756,12 +3756,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -3785,68 +3785,68 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3858,12 +3858,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3909,12 +3909,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3926,12 +3926,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -3977,12 +3977,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -3994,58 +3994,58 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -4057,12 +4057,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -4074,17 +4074,17 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -4096,12 +4096,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -4113,12 +4113,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4159,63 +4159,63 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4227,12 +4227,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4244,17 +4244,17 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4300,12 +4300,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -4317,24 +4317,24 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4346,29 +4346,29 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4380,12 +4380,12 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4397,29 +4397,29 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -4431,17 +4431,17 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -4453,12 +4453,12 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -4470,24 +4470,24 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4499,12 +4499,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4516,41 +4516,41 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4560,19 +4560,19 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4594,31 +4594,31 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4635,41 +4635,41 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -4686,46 +4686,46 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4737,12 +4737,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4754,97 +4754,97 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -4856,12 +4856,12 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -4873,97 +4873,97 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4975,12 +4975,12 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -4992,46 +4992,46 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -5043,29 +5043,29 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -5077,92 +5077,92 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -5179,12 +5179,12 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -5196,12 +5196,12 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -5213,131 +5213,131 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Helen(F)</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -5349,391 +5349,119 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Lili(F)</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Matthew(F)</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Daisy(S)</t>
+          <t>Ka(F)</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Kit(F)</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Paul(F)</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B297" t="inlineStr">
-        <is>
-          <t>Ka(F)</t>
-        </is>
-      </c>
-      <c r="C297" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B298" t="inlineStr">
-        <is>
-          <t>Kit(F)</t>
-        </is>
-      </c>
-      <c r="C298" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B299" t="inlineStr">
-        <is>
-          <t>Kit(F)</t>
-        </is>
-      </c>
-      <c r="C299" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B300" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C300" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B301" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C301" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B302" t="inlineStr">
-        <is>
-          <t>Daisy(S)</t>
-        </is>
-      </c>
-      <c r="C302" t="inlineStr">
-        <is>
-          <t>13-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B303" t="inlineStr">
-        <is>
-          <t>Helen(F)</t>
-        </is>
-      </c>
-      <c r="C303" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B304" t="inlineStr">
-        <is>
-          <t>Helen(F)</t>
-        </is>
-      </c>
-      <c r="C304" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B305" t="inlineStr">
-        <is>
-          <t>Lili(F)</t>
-        </is>
-      </c>
-      <c r="C305" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B306" t="inlineStr">
-        <is>
-          <t>Matthew(F)</t>
-        </is>
-      </c>
-      <c r="C306" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B307" t="inlineStr">
-        <is>
-          <t>Ka(F)</t>
-        </is>
-      </c>
-      <c r="C307" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B308" t="inlineStr">
-        <is>
-          <t>Kit(F)</t>
-        </is>
-      </c>
-      <c r="C308" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B309" t="inlineStr">
-        <is>
-          <t>Kit(F)</t>
-        </is>
-      </c>
-      <c r="C309" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B310" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C310" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B311" t="inlineStr">
-        <is>
-          <t>Paul(F)</t>
-        </is>
-      </c>
-      <c r="C311" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B312" t="inlineStr">
-        <is>
-          <t>Daisy(S)</t>
-        </is>
-      </c>
-      <c r="C312" t="inlineStr">
-        <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete and Name display(for consistency, no longer uses (F) for freelancers)
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -1937,7 +1937,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2770,7 +2770,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>test1(F)</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2872,7 +2872,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3042,7 +3042,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3093,7 +3093,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3195,7 +3195,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3212,7 +3212,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>test2(F)</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3824,7 +3824,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -4096,7 +4096,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -4266,7 +4266,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4402,7 +4402,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -4419,7 +4419,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -4453,7 +4453,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4504,7 +4504,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -4555,7 +4555,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -4674,7 +4674,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -4691,7 +4691,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -4708,7 +4708,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4759,7 +4759,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -4827,7 +4827,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -4895,7 +4895,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -5048,7 +5048,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -5065,7 +5065,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -5099,7 +5099,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -5201,7 +5201,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -5252,7 +5252,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -5269,7 +5269,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -5303,7 +5303,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Helen(F)</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -5354,7 +5354,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Lili(F)</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Matthew(F)</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Ka(F)</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Kit(F)</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -5439,7 +5439,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Paul(F)</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">

</xml_diff>

<commit_message>
Adding three new roles; UI: Employee List display enhanced
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C296"/>
+  <dimension ref="A1:C272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -628,24 +628,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -657,17 +657,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -827,29 +827,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,34 +861,34 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -917,12 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -968,80 +968,80 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1184,12 +1184,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1201,63 +1201,63 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1274,12 +1274,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1393,41 +1393,41 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1439,12 +1439,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1456,34 +1456,34 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1592,46 +1592,46 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1643,51 +1643,51 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1750,24 +1750,24 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1779,97 +1779,97 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1881,29 +1881,29 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1915,29 +1915,29 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1949,63 +1949,63 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2017,7 +2017,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2027,19 +2027,19 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2051,7 +2051,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2061,36 +2061,36 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2102,29 +2102,29 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2136,29 +2136,29 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2170,12 +2170,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2187,29 +2187,29 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2221,12 +2221,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2238,92 +2238,92 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2340,29 +2340,29 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2374,29 +2374,29 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2408,12 +2408,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2425,12 +2425,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2442,12 +2442,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2459,46 +2459,46 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2510,29 +2510,29 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2544,7 +2544,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2554,87 +2554,87 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2646,80 +2646,80 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2731,80 +2731,80 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2816,12 +2816,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -2833,7 +2833,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2843,14 +2843,14 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2867,7 +2867,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2884,63 +2884,63 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2952,12 +2952,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2969,12 +2969,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3003,97 +3003,97 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3105,29 +3105,29 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3139,63 +3139,63 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -3207,12 +3207,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3224,126 +3224,126 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3360,7 +3360,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -3370,14 +3370,14 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -3387,31 +3387,31 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -3421,31 +3421,31 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -3455,14 +3455,14 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -3472,53 +3472,53 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3530,12 +3530,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3547,12 +3547,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3564,29 +3564,29 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3598,46 +3598,46 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3649,12 +3649,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3666,7 +3666,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -3676,172 +3676,172 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3853,46 +3853,46 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3904,12 +3904,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3921,63 +3921,63 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -3989,63 +3989,63 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -4057,12 +4057,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -4074,80 +4074,80 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4159,29 +4159,29 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4193,12 +4193,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4210,29 +4210,29 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4244,46 +4244,46 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4295,7 +4295,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4305,36 +4305,36 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4346,12 +4346,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4363,29 +4363,29 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4397,29 +4397,29 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -4431,12 +4431,12 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -4448,29 +4448,29 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4482,29 +4482,29 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4516,199 +4516,199 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4720,12 +4720,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4737,29 +4737,29 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4771,63 +4771,63 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -4839,63 +4839,63 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -4907,12 +4907,12 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -4924,29 +4924,29 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4958,12 +4958,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -4975,12 +4975,12 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -4992,12 +4992,12 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -5009,24 +5009,24 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -5043,7 +5043,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -5052,414 +5052,6 @@
         </is>
       </c>
       <c r="C272" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C273" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>Lili</t>
-        </is>
-      </c>
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B276" t="inlineStr">
-        <is>
-          <t>Ka</t>
-        </is>
-      </c>
-      <c r="C276" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B277" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C277" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
-      </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C278" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C279" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B280" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C280" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>Lili</t>
-        </is>
-      </c>
-      <c r="C281" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>Matthew</t>
-        </is>
-      </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B283" t="inlineStr">
-        <is>
-          <t>Ka</t>
-        </is>
-      </c>
-      <c r="C283" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B284" t="inlineStr">
-        <is>
-          <t>Kit</t>
-        </is>
-      </c>
-      <c r="C284" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B285" t="inlineStr">
-        <is>
-          <t>Kit</t>
-        </is>
-      </c>
-      <c r="C285" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B286" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B287" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C287" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B288" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C288" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B289" t="inlineStr">
-        <is>
-          <t>Helen</t>
-        </is>
-      </c>
-      <c r="C289" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B290" t="inlineStr">
-        <is>
-          <t>Lili</t>
-        </is>
-      </c>
-      <c r="C290" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>Matthew</t>
-        </is>
-      </c>
-      <c r="C291" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B292" t="inlineStr">
-        <is>
-          <t>Ka</t>
-        </is>
-      </c>
-      <c r="C292" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B293" t="inlineStr">
-        <is>
-          <t>Kit</t>
-        </is>
-      </c>
-      <c r="C293" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B294" t="inlineStr">
-        <is>
-          <t>Kit</t>
-        </is>
-      </c>
-      <c r="C294" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B295" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C295" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
-      </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>Paul</t>
-        </is>
-      </c>
-      <c r="C296" t="inlineStr">
         <is>
           <t>7-16</t>
         </is>

</xml_diff>

<commit_message>
Precautionary bug fix: get_available_shifts for Class Freelancer
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C272"/>
+  <dimension ref="A1:C279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -640,17 +640,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -827,12 +827,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -844,17 +844,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -883,12 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -917,12 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -934,12 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -968,63 +968,63 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1087,12 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1172,41 +1172,41 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1218,34 +1218,34 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-03-21</t>
+          <t>2025-03-20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1393,97 +1393,97 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2025-03-21</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1512,12 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1592,46 +1592,46 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1643,51 +1643,51 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-22</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1750,24 +1750,24 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1779,102 +1779,102 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1886,12 +1886,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1903,24 +1903,24 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -1932,12 +1932,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1949,46 +1949,46 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2000,7 +2000,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2010,24 +2010,24 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -2039,12 +2039,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2068,58 +2068,58 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2136,7 +2136,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2146,14 +2146,14 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2163,14 +2163,14 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-03-26</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2180,70 +2180,70 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2255,7 +2255,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2265,31 +2265,31 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -2311,75 +2311,75 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2391,29 +2391,29 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2425,17 +2425,17 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2025-03-27</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -2447,12 +2447,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2464,19 +2464,19 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2486,14 +2486,14 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2510,7 +2510,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2520,87 +2520,87 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-03-29</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-28</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2612,29 +2612,29 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2646,24 +2646,24 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-29</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2685,121 +2685,121 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -2821,36 +2821,36 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2860,31 +2860,31 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2901,7 +2901,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2911,31 +2911,31 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2025-03-31</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2969,12 +2969,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2986,58 +2986,58 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -3047,41 +3047,41 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3093,12 +3093,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3110,24 +3110,24 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3139,29 +3139,29 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3173,12 +3173,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3190,29 +3190,29 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -3224,17 +3224,17 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-04-02</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -3263,12 +3263,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3314,12 +3314,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3331,12 +3331,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3348,12 +3348,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3365,24 +3365,24 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3394,12 +3394,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3411,63 +3411,63 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3479,17 +3479,17 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-04-04</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3501,12 +3501,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3518,12 +3518,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3535,12 +3535,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3552,12 +3552,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3569,12 +3569,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3586,53 +3586,53 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3642,19 +3642,19 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3666,29 +3666,29 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3700,17 +3700,17 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -3722,12 +3722,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3751,114 +3751,114 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -3875,12 +3875,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -3892,7 +3892,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3921,119 +3921,119 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-04-07</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -4045,12 +4045,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -4062,24 +4062,24 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -4091,58 +4091,58 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -4152,31 +4152,31 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2025-04-07</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -4186,7 +4186,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -4220,14 +4220,14 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -4244,58 +4244,58 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -4312,29 +4312,29 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-08</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4346,58 +4346,58 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -4414,24 +4414,24 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -4441,14 +4441,14 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -4465,7 +4465,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -4475,14 +4475,14 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -4499,7 +4499,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -4509,14 +4509,14 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-10</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -4526,14 +4526,14 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -4550,7 +4550,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -4560,14 +4560,14 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -4584,7 +4584,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -4601,7 +4601,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -4618,7 +4618,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -4628,14 +4628,14 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -4645,14 +4645,14 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -4669,7 +4669,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -4686,7 +4686,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -4703,12 +4703,12 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4720,24 +4720,24 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -4747,31 +4747,31 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -4788,41 +4788,41 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -4839,34 +4839,34 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -4878,12 +4878,12 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -4895,58 +4895,58 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -4958,68 +4958,68 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -5031,12 +5031,12 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -5048,12 +5048,131 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Lili</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Matthew</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>0930-1830</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Ka</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Kit</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Kit</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>0930-1830</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fixed: correct shift button color; imported shift time now overrides customized shift time
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C533"/>
+  <dimension ref="A1:C532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8346,12 +8346,12 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -8363,29 +8363,29 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Caper</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>Caper</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -8402,7 +8402,7 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
@@ -8465,12 +8465,12 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -8482,12 +8482,12 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -8499,12 +8499,12 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -8521,7 +8521,7 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -8538,7 +8538,7 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -8550,12 +8550,12 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Waiyee</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8567,12 +8567,12 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>Waiyee</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -8584,12 +8584,12 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -8601,12 +8601,12 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Aasta</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8618,12 +8618,12 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>Aasta</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -8635,12 +8635,12 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Jackie</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -8652,12 +8652,12 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>Jackie</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8669,12 +8669,12 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -8686,12 +8686,12 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -8703,29 +8703,29 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Caper</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>2025-04-11</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Caper</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -8742,7 +8742,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8759,7 +8759,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -8771,12 +8771,12 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Matthew</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -8793,7 +8793,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8810,7 +8810,7 @@
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -8822,12 +8822,12 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Waiyee</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -8839,12 +8839,12 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>Waiyee</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -8856,12 +8856,12 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>自由調配</t>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -8873,12 +8873,12 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Aasta</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -8890,12 +8890,12 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Aasta</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -8907,12 +8907,12 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Jackie</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -8924,12 +8924,12 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Jackie</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -8941,12 +8941,12 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -8958,29 +8958,29 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>自由調配</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -8992,7 +8992,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Lili</t>
         </is>
       </c>
       <c r="C504" t="inlineStr">
@@ -9009,12 +9009,12 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Lili</t>
+          <t>Waiyee</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -9026,12 +9026,12 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Waiyee</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9043,7 +9043,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -9060,12 +9060,12 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Aasta</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -9077,12 +9077,12 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>Aasta</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -9094,12 +9094,12 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Jackie</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>自由調配</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9111,12 +9111,12 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Jackie</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -9128,12 +9128,12 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -9145,29 +9145,29 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
         </is>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Helen</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>0930-1830</t>
         </is>
       </c>
     </row>
@@ -9179,12 +9179,12 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Helen</t>
+          <t>Waiyee</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -9196,12 +9196,12 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Waiyee</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9213,7 +9213,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
@@ -9230,12 +9230,12 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Aasta</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -9247,12 +9247,12 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>Aasta</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">
         <is>
-          <t>自由調配</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9264,7 +9264,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Jackie</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>Jackie</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
@@ -9298,12 +9298,12 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C522" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -9315,29 +9315,29 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C523" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>2025-04-14</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>Tak</t>
+          <t>Waiyee</t>
         </is>
       </c>
       <c r="C524" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9349,12 +9349,12 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>Waiyee</t>
+          <t>Cindy</t>
         </is>
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -9366,12 +9366,12 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>Cindy</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C526" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -9383,12 +9383,12 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Aasta</t>
         </is>
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9400,7 +9400,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>Aasta</t>
+          <t>Carol</t>
         </is>
       </c>
       <c r="C528" t="inlineStr">
@@ -9417,12 +9417,12 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>Carol</t>
+          <t>Jackie</t>
         </is>
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -9434,12 +9434,12 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>Jackie</t>
+          <t>Tiffany</t>
         </is>
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -9451,12 +9451,12 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -9468,27 +9468,10 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Tak</t>
         </is>
       </c>
       <c r="C532" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" t="inlineStr">
-        <is>
-          <t>2025-04-17</t>
-        </is>
-      </c>
-      <c r="B533" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-      <c r="C533" t="inlineStr">
         <is>
           <t>自由調配</t>
         </is>

</xml_diff>

<commit_message>
exporting schedule/availability with file explorer
</commit_message>
<xml_diff>
--- a/availability_export.xlsx
+++ b/availability_export.xlsx
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -7943,7 +7943,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -8572,7 +8572,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -9422,7 +9422,7 @@
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="C541" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>

</xml_diff>